<commit_message>
enhanced the FaceSecure project by fixing errors, ensuring robust Excel data handling, and implementing automatic cleanup to limit captured images to 5 for efficient memory usage.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -432,54 +432,46 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="23" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>S.No</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Identified Person</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Entry Time_2025-01-24</t>
+          <t>Entry Time</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Exit Time_2025-01-24</t>
+          <t>Exit Time</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-01-27</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mehar</t>
+          <t>Meharjot</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>22:55:39</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>22:55:48</t>
-        </is>
-      </c>
+          <t>18:47:06</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>